<commit_message>
Excel reader utilites fixed
</commit_message>
<xml_diff>
--- a/Tricentis/com/Tricenties/testData/VehicleInsuranceCalcualator_TestData.xlsx
+++ b/Tricentis/com/Tricenties/testData/VehicleInsuranceCalcualator_TestData.xlsx
@@ -1,24 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\eclipse-workspace\Training.InsuranceCalculator\src\test\resources\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0788422-D740-4539-B247-27CABBD8CD2F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A380FA76-9CC6-4F4D-9280-5EC28A377BCB}"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15090" windowHeight="3525"/>
   </bookViews>
   <sheets>
     <sheet name="InsurancePremium" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1:F8"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -274,8 +269,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,7 +422,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -479,7 +474,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -673,45 +668,45 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{255CEB0C-D017-479D-8DDE-08C67B4AF72D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="41.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="18" width="19.77734375" customWidth="1"/>
-    <col min="19" max="19" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="19.77734375" customWidth="1"/>
-    <col min="22" max="22" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.44140625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="18" width="19.7109375" customWidth="1"/>
+    <col min="19" max="19" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="19.7109375" customWidth="1"/>
+    <col min="22" max="22" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.42578125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -797,7 +792,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28">
       <c r="A2">
         <v>1</v>
       </c>
@@ -883,7 +878,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28">
       <c r="A3">
         <v>2</v>
       </c>
@@ -969,7 +964,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1062,16 +1057,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E0B929-9698-4D94-8FD9-1582B0293DA0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="115" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -1079,7 +1074,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1087,7 +1082,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>74</v>
       </c>

</xml_diff>